<commit_message>
Excel still being completed + FeatureFunction use simplified with Enums
</commit_message>
<xml_diff>
--- a/excel/results_FeatureFonctions.xlsx
+++ b/excel/results_FeatureFonctions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\A-DOCS\Polytech\4A\ISI3\ia-4a-tpmdp-ensuque\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ensuque\Documents\1-TRUE DOCUMENTS\Polytech\4A\ISI3\TP1\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B22E117-B8F6-4D35-92BD-FEE399D4F189}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60BB4F1-94FD-4318-B033-D3DAF0C7AFEC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{227635A9-40B6-4196-97DE-A258BE6D7277}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{227635A9-40B6-4196-97DE-A258BE6D7277}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Features Fonctions choisis</t>
   </si>
@@ -235,6 +235,483 @@
   </si>
   <si>
     <r>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">s, a)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(sans biais)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">~% de succès sur </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mediumGrid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">~% de succès sur </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SmallGrid2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">~% de succès sur </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SmallGrid</t>
+    </r>
+  </si>
+  <si>
+    <t>Esquive-man</t>
+  </si>
+  <si>
+    <r>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(s, a),
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(biais + nbGhostProche)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a)
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>biais + hasDot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>43%
+SCORES NEGATIF</t>
+  </si>
+  <si>
+    <t>Nombre de fantômes qui peuvent atteindre en quatre pas ou moins la future position du pacman.</t>
+  </si>
+  <si>
+    <r>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s, a), φ4(s, a)
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>biais + hasDot + distance + nbGhostDist3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>7%
+(2 - 21%)</t>
+  </si>
+  <si>
+    <t>Distance fantôme le plus proche sur la nouvelle position.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dist(s,a) / (mapX + mapY)</t>
+  </si>
+  <si>
+    <r>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s, a)
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>biais + nbGhostProche +  hasDot + distanceDot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">φ0(s, a), φ1(s, a), φ2(s, a), 
 </t>
     </r>
@@ -247,8 +724,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(sans distance)</t>
-    </r>
+      <t>(sans distanceDot)</t>
+    </r>
+  </si>
+  <si>
+    <t>Haute variance sur les graphes</t>
   </si>
   <si>
     <r>
@@ -263,6 +743,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>1</t>
     </r>
     <r>
@@ -315,8 +816,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">s, a)
-</t>
+      <t>s, a),φ4(s, a), φ5(s, a) 
+(</t>
     </r>
     <r>
       <rPr>
@@ -327,12 +828,86 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(sans biais)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">~% de succès sur </t>
+      <t>Tous!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a)
+(</t>
     </r>
     <r>
       <rPr>
@@ -343,12 +918,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>mediumGrid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">~% de succès sur </t>
+      <t xml:space="preserve">biais + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nbGhostDist3</t>
     </r>
     <r>
       <rPr>
@@ -359,23 +939,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>SmallGrid2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">~% de succès sur </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SmallGrid</t>
+      <t xml:space="preserve"> +  hasDot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
   <si>
@@ -443,18 +1017,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(s, a), φ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3(</t>
+      <t>(s, a), φ5</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
     </r>
     <r>
       <rPr>
@@ -476,72 +1050,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>biais + nbGhostProche +  hasDot + distance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>43%
-SCORE NEGATIF</t>
-  </si>
-  <si>
-    <t>Esquive-man</t>
-  </si>
-  <si>
-    <r>
-      <t>φ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(s, a), φ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(s, a),
-</t>
+      <t xml:space="preserve">biais + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nbGhostProche</t>
     </r>
     <r>
       <rPr>
@@ -552,66 +1071,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(biais + nbGhostProche)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>φ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(s, a), φ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(s, a)
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>biais + hasDot</t>
+      <t xml:space="preserve"> + nbGhostDist3 +  hasDot</t>
     </r>
     <r>
       <rPr>
@@ -700,9 +1160,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -711,6 +1168,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1026,9 +1486,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E22599B-B8A4-49E2-8DD2-C6B6769DF984}">
-  <dimension ref="B3:N22"/>
+  <dimension ref="B3:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1037,10 +1497,10 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="40" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="9" width="15.42578125" customWidth="1"/>
     <col min="12" max="12" width="28.7109375" customWidth="1"/>
   </cols>
@@ -1065,30 +1525,33 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1"/>
+      <c r="I4" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="2:14" ht="48" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6">
         <v>0.86</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>0.8</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>0.5</v>
       </c>
       <c r="J5" s="1"/>
@@ -1097,16 +1560,16 @@
     </row>
     <row r="6" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
-      <c r="D6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6">
         <v>0.83</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>0.87</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>0.56000000000000005</v>
       </c>
       <c r="J6" s="1"/>
@@ -1115,58 +1578,58 @@
     </row>
     <row r="7" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6">
         <v>0.97</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>0.88</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
-      <c r="D8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="6">
         <v>0.85</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>0.81</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="7"/>
       <c r="J8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-      <c r="D9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6">
         <v>0</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>0</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>0</v>
       </c>
       <c r="H9" s="2"/>
@@ -1175,24 +1638,40 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="D10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.3</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="D11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.63</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.3</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="1"/>
@@ -1201,86 +1680,83 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+    <row r="12" spans="2:14" ht="33" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.94</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="2:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+    <row r="13" spans="2:14" ht="33" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+    <row r="16" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1289,13 +1765,17 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="2:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+    <row r="17" spans="2:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1304,13 +1784,16 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1319,10 +1802,13 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+    <row r="19" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1333,10 +1819,13 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+    <row r="20" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1347,10 +1836,13 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+    <row r="21" spans="2:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1361,10 +1853,16 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+    <row r="22" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1375,6 +1873,66 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ongoing QLearning testing (excels) + simplified EtatMap criteria choice with Enum
</commit_message>
<xml_diff>
--- a/excel/results_FeatureFonctions.xlsx
+++ b/excel/results_FeatureFonctions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ensuque\Documents\1-TRUE DOCUMENTS\Polytech\4A\ISI3\TP1\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60BB4F1-94FD-4318-B033-D3DAF0C7AFEC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ED4E50-7231-45FD-AF86-8C7882B4AC0D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{227635A9-40B6-4196-97DE-A258BE6D7277}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Features Fonctions choisis</t>
   </si>
@@ -1083,6 +1083,258 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ5</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s, a)
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">biais + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DistClose</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + nbGhostDist3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <r>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s, a), φ5</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s, a)
+(distanceGhost</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + nbGhostDist3 +  hasDot + distanceDot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Manhattan est désatreux</t>
+  </si>
+  <si>
+    <t>Diviser les distances</t>
   </si>
 </sst>
 </file>
@@ -1486,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E22599B-B8A4-49E2-8DD2-C6B6769DF984}">
-  <dimension ref="B3:N28"/>
+  <dimension ref="B3:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +1764,9 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1554,6 +1808,9 @@
       <c r="G5" s="6">
         <v>0.5</v>
       </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -1571,6 +1828,9 @@
       </c>
       <c r="G6" s="6">
         <v>0.56000000000000005</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
       </c>
       <c r="J6" s="1"/>
       <c r="M6" s="1"/>
@@ -1705,11 +1965,17 @@
     <row r="13" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.01</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="1"/>
@@ -1718,12 +1984,20 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="48" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="D14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.7</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="1"/>
@@ -1732,12 +2006,20 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="D15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.93</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.74</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.8</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="1"/>
@@ -1791,6 +2073,7 @@
       <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D18" s="9"/>
       <c r="E18" s="8"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -1809,6 +2092,7 @@
       <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D19" s="9"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1859,9 +2143,6 @@
       </c>
       <c r="C22" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1888,6 +2169,9 @@
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1901,7 +2185,6 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1915,7 +2198,6 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1933,6 +2215,12 @@
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
     </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>